<commit_message>
Adding Header, Main, Scetion and Footer elements and ALT modifications for images
</commit_message>
<xml_diff>
--- a/Audit-SEO-LaChouette-HZ.xlsx
+++ b/Audit-SEO-LaChouette-HZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OpenClassroom\P4_Zoubeiri_Housna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882A33BC-B0C4-44E6-8CF2-A755C17C2D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4610A7-F656-489D-9B8F-23B1FCA965BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analyse" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="160">
   <si>
     <t>Catégorie</t>
   </si>
@@ -155,15 +155,6 @@
     <t>avec bonne localisation</t>
   </si>
   <si>
-    <t>Header, Main et Footer</t>
-  </si>
-  <si>
-    <t>Absence de balises sémantiques</t>
-  </si>
-  <si>
-    <t>et barre navigation</t>
-  </si>
-  <si>
     <t>Image background trop lourde en bmp</t>
   </si>
   <si>
@@ -212,9 +203,6 @@
     <t>en intégrant mot-clé relative à l'activité"web design"</t>
   </si>
   <si>
-    <t>ne contient pas de mots-clé</t>
-  </si>
-  <si>
     <t xml:space="preserve">  relative à l'activité</t>
   </si>
   <si>
@@ -227,12 +215,6 @@
     <t xml:space="preserve">Ajouter "Web " et "design" au contenu de H1 </t>
   </si>
   <si>
-    <t>trop long</t>
-  </si>
-  <si>
-    <t>Réduire h2 pour être attractif et avec mot-clé</t>
-  </si>
-  <si>
     <t xml:space="preserve">Titre H2 </t>
   </si>
   <si>
@@ -413,9 +395,6 @@
     <t xml:space="preserve">et placer le site sous le nom de domaine </t>
   </si>
   <si>
-    <t>Placer le site sous le nom de domaine de l'agence</t>
-  </si>
-  <si>
     <t>"lachouetteagence.com"</t>
   </si>
   <si>
@@ -510,6 +489,30 @@
   </si>
   <si>
     <t>Kwfinder</t>
+  </si>
+  <si>
+    <t>Enlever le point et ajouter un mots-clé</t>
+  </si>
+  <si>
+    <t>Paramétrer URL</t>
+  </si>
+  <si>
+    <t>Police et couleur pas assez contrasté</t>
+  </si>
+  <si>
+    <t>Renseigner un texte alternatif à l'image</t>
+  </si>
+  <si>
+    <t>Absence de balises de structures</t>
+  </si>
+  <si>
+    <t>Header, Main , Section et Footer</t>
+  </si>
+  <si>
+    <t>Police différente du reste du texte</t>
+  </si>
+  <si>
+    <t>Police et couleur pas assez contrastée</t>
   </si>
 </sst>
 </file>
@@ -867,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1042"/>
+  <dimension ref="A1:Z1044"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -933,7 +936,7 @@
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4"/>
     </row>
@@ -943,7 +946,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -952,10 +955,10 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -963,31 +966,31 @@
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E8" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E9" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E10" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -995,31 +998,31 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1037,7 +1040,7 @@
         <v>25</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1057,10 +1060,10 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="E20" s="6"/>
     </row>
@@ -1071,38 +1074,38 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E24" s="6"/>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B25" s="5"/>
       <c r="E25" s="7"/>
@@ -1110,30 +1113,30 @@
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E28" s="7"/>
     </row>
@@ -1141,7 +1144,7 @@
       <c r="A29" s="3"/>
       <c r="B29" s="5"/>
       <c r="C29" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E29" s="7"/>
     </row>
@@ -1167,7 +1170,7 @@
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1181,12 +1184,12 @@
         <v>10</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E34" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1222,7 +1225,7 @@
         <v>11</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1243,12 +1246,12 @@
     </row>
     <row r="44" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E44" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E45" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1261,347 +1264,368 @@
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="B49" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="D49" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C50" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="A52" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="8"/>
       <c r="E53" s="6"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="C54" t="s">
-        <v>40</v>
+        <v>154</v>
+      </c>
+      <c r="D54" t="s">
+        <v>158</v>
       </c>
       <c r="E54" s="6"/>
     </row>
     <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
-        <v>42</v>
-      </c>
       <c r="E55" s="6"/>
     </row>
     <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" t="s">
+        <v>157</v>
+      </c>
       <c r="E56" s="6"/>
     </row>
     <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="s">
         <v>30</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>34</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="D59" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" t="s">
-        <v>37</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E61" s="6"/>
+      <c r="C61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E63" s="6"/>
     </row>
     <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E64" s="6"/>
+      <c r="C64" t="s">
+        <v>40</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" t="s">
-        <v>46</v>
-      </c>
-      <c r="C65" t="s">
-        <v>52</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C66" t="s">
-        <v>47</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>47</v>
-      </c>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B67" t="s">
+        <v>43</v>
+      </c>
       <c r="C67" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C68" s="6" t="s">
-        <v>70</v>
+      <c r="C68" t="s">
+        <v>44</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E69" s="6"/>
+      <c r="C69" t="s">
+        <v>45</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E70" s="6"/>
+      <c r="C70" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" t="s">
+        <v>84</v>
+      </c>
+      <c r="E73" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E71" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C73" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E74" s="6"/>
+      <c r="B74" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E75" s="6"/>
+      <c r="C75" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E76" s="6"/>
     </row>
     <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
+      <c r="B77" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E77" s="6"/>
-    </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B78" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C79" s="6" t="s">
-        <v>73</v>
+      <c r="B79" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E80" s="6"/>
+      <c r="B80" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B81" t="s">
+      <c r="C81" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83" t="s">
+        <v>88</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C84" t="s">
         <v>89</v>
       </c>
-      <c r="C81" t="s">
-        <v>94</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C82" t="s">
-        <v>95</v>
-      </c>
-      <c r="E82" s="6"/>
-    </row>
-    <row r="83" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E83" s="6"/>
-    </row>
-    <row r="84" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E84" s="6"/>
     </row>
     <row r="85" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="E85" s="6"/>
     </row>
     <row r="86" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E86" s="6"/>
     </row>
     <row r="87" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="E87" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E88" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="E88" s="6"/>
     </row>
     <row r="89" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E89" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E90" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E91" s="6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E92" s="6"/>
+      <c r="E92" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="93" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E93" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E94" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="E94" s="6"/>
     </row>
     <row r="95" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E95" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E96" s="6" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E97" s="6"/>
+      <c r="E97" s="6" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="98" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E98" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E99" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="E99" s="6"/>
     </row>
     <row r="100" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E100" s="6"/>
+      <c r="E100" s="6" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="101" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E101" s="6"/>
+      <c r="E101" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="102" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="8" t="s">
-        <v>102</v>
-      </c>
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E104" s="6"/>
+    </row>
+    <row r="105" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E105" s="6"/>
+    </row>
     <row r="106" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="107" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="108" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2539,6 +2563,8 @@
     <row r="1040" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1041" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="1042" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1043" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="1044" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -2560,60 +2586,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2629,7 +2655,7 @@
   </sheetPr>
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2642,43 +2668,43 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B2" s="15">
         <v>200</v>
       </c>
       <c r="C2" s="11"/>
       <c r="E2" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B3" s="15">
         <v>890</v>
       </c>
       <c r="C3" s="11"/>
       <c r="E3" s="14" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2688,19 +2714,19 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -2712,7 +2738,7 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B9" s="11">
         <v>170</v>
@@ -2721,7 +2747,7 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
@@ -2733,21 +2759,21 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>